<commit_message>
Testing the different data point
</commit_message>
<xml_diff>
--- a/soft.xlsx
+++ b/soft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15149eb1c9cf386c/Escritorio/TFG/Codigo-GIT/TFG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_FFC65FC0A2996DC0B2160BEE936B717A4534E702" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE11909D-6508-410C-A4A4-F190745416C3}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_FFC65FC0A2996DC0B2160BEE936B717A4534E702" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F9ECADA-6A42-49E3-8C47-845752580284}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D75"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2035,7 +2035,7 @@
         <v>8.1056516774969539E-4</v>
       </c>
       <c r="D75">
-        <f t="shared" si="3"/>
+        <f>B75/1.4765679173556 * 10^(-4)</f>
         <v>2.578431287116853E-4</v>
       </c>
     </row>

</xml_diff>